<commit_message>
Fix errors in the annotation
</commit_message>
<xml_diff>
--- a/harana/datasets/BPSFH/18/chords.xlsx
+++ b/harana/datasets/BPSFH/18/chords.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iis519\Desktop\Dataset\BPS Dataset\18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiaoyu/Desktop/video_music/harana/harana/datasets/BPSFH/18/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE554A1C-3C96-4144-8957-42D5FA7CE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12396"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -366,14 +367,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>a6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fr+6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -502,26 +495,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>5/5</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>V43/V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -597,7 +595,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -874,19 +872,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="G193" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="A201" sqref="A201:G205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="7" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -909,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>9</v>
       </c>
@@ -932,7 +930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>15</v>
       </c>
@@ -955,7 +953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>18</v>
       </c>
@@ -978,7 +976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -1001,7 +999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>27</v>
       </c>
@@ -1024,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>36</v>
       </c>
@@ -1047,7 +1045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42</v>
       </c>
@@ -1070,7 +1068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45</v>
       </c>
@@ -1093,7 +1091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>48</v>
       </c>
@@ -1116,7 +1114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>51</v>
       </c>
@@ -1139,7 +1137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>54</v>
       </c>
@@ -1162,7 +1160,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>57</v>
       </c>
@@ -1185,7 +1183,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>59</v>
       </c>
@@ -1208,7 +1206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>60</v>
       </c>
@@ -1231,7 +1229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>63</v>
       </c>
@@ -1254,7 +1252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>66</v>
       </c>
@@ -1277,7 +1275,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>69</v>
       </c>
@@ -1300,7 +1298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>71</v>
       </c>
@@ -1323,7 +1321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>72</v>
       </c>
@@ -1346,7 +1344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>75</v>
       </c>
@@ -1369,7 +1367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>78</v>
       </c>
@@ -1392,7 +1390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>81</v>
       </c>
@@ -1415,7 +1413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>84</v>
       </c>
@@ -1438,7 +1436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>87</v>
       </c>
@@ -1461,7 +1459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>90</v>
       </c>
@@ -1484,7 +1482,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>96</v>
       </c>
@@ -1507,7 +1505,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>104</v>
       </c>
@@ -1530,7 +1528,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>105</v>
       </c>
@@ -1553,7 +1551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>107</v>
       </c>
@@ -1576,7 +1574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>108</v>
       </c>
@@ -1599,7 +1597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>110</v>
       </c>
@@ -1622,7 +1620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>111</v>
       </c>
@@ -1645,7 +1643,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>113</v>
       </c>
@@ -1668,7 +1666,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>114</v>
       </c>
@@ -1691,7 +1689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>116</v>
       </c>
@@ -1714,7 +1712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>117</v>
       </c>
@@ -1737,7 +1735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>119</v>
       </c>
@@ -1760,7 +1758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>120</v>
       </c>
@@ -1783,7 +1781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>122</v>
       </c>
@@ -1806,7 +1804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>123</v>
       </c>
@@ -1829,7 +1827,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>125</v>
       </c>
@@ -1852,7 +1850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>126</v>
       </c>
@@ -1875,7 +1873,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>129</v>
       </c>
@@ -1898,7 +1896,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>135</v>
       </c>
@@ -1921,7 +1919,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>141</v>
       </c>
@@ -1944,7 +1942,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>144</v>
       </c>
@@ -1967,7 +1965,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>146</v>
       </c>
@@ -1990,7 +1988,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>147</v>
       </c>
@@ -2013,7 +2011,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>152</v>
       </c>
@@ -2036,7 +2034,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>153</v>
       </c>
@@ -2059,7 +2057,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>154</v>
       </c>
@@ -2082,7 +2080,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>155</v>
       </c>
@@ -2105,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>156</v>
       </c>
@@ -2128,7 +2126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>168</v>
       </c>
@@ -2151,7 +2149,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>174</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>177</v>
       </c>
@@ -2197,7 +2195,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>179</v>
       </c>
@@ -2220,7 +2218,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>180</v>
       </c>
@@ -2243,7 +2241,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>185</v>
       </c>
@@ -2266,7 +2264,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>186</v>
       </c>
@@ -2289,7 +2287,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>187</v>
       </c>
@@ -2312,7 +2310,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>188</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>189</v>
       </c>
@@ -2358,7 +2356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>192</v>
       </c>
@@ -2381,7 +2379,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>195</v>
       </c>
@@ -2404,7 +2402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>198</v>
       </c>
@@ -2427,7 +2425,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>201</v>
       </c>
@@ -2450,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>202</v>
       </c>
@@ -2473,7 +2471,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>203</v>
       </c>
@@ -2496,7 +2494,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>204</v>
       </c>
@@ -2519,7 +2517,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>205</v>
       </c>
@@ -2542,7 +2540,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>206</v>
       </c>
@@ -2565,7 +2563,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>207</v>
       </c>
@@ -2588,7 +2586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>208</v>
       </c>
@@ -2611,7 +2609,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>209</v>
       </c>
@@ -2634,7 +2632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>210</v>
       </c>
@@ -2657,7 +2655,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>211</v>
       </c>
@@ -2680,7 +2678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>212</v>
       </c>
@@ -2703,7 +2701,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>213</v>
       </c>
@@ -2726,7 +2724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>231</v>
       </c>
@@ -2749,7 +2747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>243</v>
       </c>
@@ -2772,7 +2770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>246</v>
       </c>
@@ -2795,7 +2793,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>249</v>
       </c>
@@ -2818,7 +2816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>252</v>
       </c>
@@ -2841,7 +2839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>255</v>
       </c>
@@ -2864,7 +2862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>258</v>
       </c>
@@ -2887,7 +2885,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>264</v>
       </c>
@@ -2910,7 +2908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>273</v>
       </c>
@@ -2933,7 +2931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>279</v>
       </c>
@@ -2956,7 +2954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>282</v>
       </c>
@@ -2979,7 +2977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>285</v>
       </c>
@@ -3002,7 +3000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>291</v>
       </c>
@@ -3025,7 +3023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>300</v>
       </c>
@@ -3048,7 +3046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>306</v>
       </c>
@@ -3071,7 +3069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>309</v>
       </c>
@@ -3094,7 +3092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>312</v>
       </c>
@@ -3117,7 +3115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>315</v>
       </c>
@@ -3140,7 +3138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>318</v>
       </c>
@@ -3163,7 +3161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>321</v>
       </c>
@@ -3186,7 +3184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>323</v>
       </c>
@@ -3209,7 +3207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>324</v>
       </c>
@@ -3232,7 +3230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>327</v>
       </c>
@@ -3255,7 +3253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>330</v>
       </c>
@@ -3278,7 +3276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>333</v>
       </c>
@@ -3301,7 +3299,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>335</v>
       </c>
@@ -3324,7 +3322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>336</v>
       </c>
@@ -3347,7 +3345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>339</v>
       </c>
@@ -3370,7 +3368,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>342</v>
       </c>
@@ -3393,7 +3391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>345</v>
       </c>
@@ -3416,7 +3414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>348</v>
       </c>
@@ -3439,7 +3437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>351</v>
       </c>
@@ -3462,7 +3460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>354</v>
       </c>
@@ -3485,7 +3483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>360</v>
       </c>
@@ -3508,7 +3506,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>368</v>
       </c>
@@ -3531,7 +3529,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>369</v>
       </c>
@@ -3554,7 +3552,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>371</v>
       </c>
@@ -3577,7 +3575,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>372</v>
       </c>
@@ -3600,7 +3598,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>374</v>
       </c>
@@ -3623,7 +3621,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>375</v>
       </c>
@@ -3646,7 +3644,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>377</v>
       </c>
@@ -3669,7 +3667,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>378</v>
       </c>
@@ -3692,7 +3690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>380</v>
       </c>
@@ -3715,7 +3713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>381</v>
       </c>
@@ -3738,7 +3736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>383</v>
       </c>
@@ -3761,7 +3759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>384</v>
       </c>
@@ -3784,7 +3782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>386</v>
       </c>
@@ -3807,7 +3805,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>387</v>
       </c>
@@ -3830,7 +3828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>389</v>
       </c>
@@ -3853,7 +3851,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>390</v>
       </c>
@@ -3876,7 +3874,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>393</v>
       </c>
@@ -3899,7 +3897,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>399</v>
       </c>
@@ -3922,7 +3920,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>405</v>
       </c>
@@ -3945,7 +3943,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>408</v>
       </c>
@@ -3968,7 +3966,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>410</v>
       </c>
@@ -3991,7 +3989,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>411</v>
       </c>
@@ -4014,7 +4012,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>416</v>
       </c>
@@ -4037,7 +4035,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>417</v>
       </c>
@@ -4060,7 +4058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>418</v>
       </c>
@@ -4083,7 +4081,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>419</v>
       </c>
@@ -4106,7 +4104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>420</v>
       </c>
@@ -4129,7 +4127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>432</v>
       </c>
@@ -4152,7 +4150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>438</v>
       </c>
@@ -4175,7 +4173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>441</v>
       </c>
@@ -4198,7 +4196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>443</v>
       </c>
@@ -4221,7 +4219,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>444</v>
       </c>
@@ -4244,7 +4242,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>449</v>
       </c>
@@ -4267,7 +4265,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>450</v>
       </c>
@@ -4290,7 +4288,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>451</v>
       </c>
@@ -4313,7 +4311,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>452</v>
       </c>
@@ -4336,7 +4334,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>453</v>
       </c>
@@ -4359,7 +4357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>456</v>
       </c>
@@ -4382,7 +4380,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>459</v>
       </c>
@@ -4405,7 +4403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>462</v>
       </c>
@@ -4428,7 +4426,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>465</v>
       </c>
@@ -4451,7 +4449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>466</v>
       </c>
@@ -4474,7 +4472,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>467</v>
       </c>
@@ -4497,7 +4495,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>468</v>
       </c>
@@ -4520,7 +4518,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>469</v>
       </c>
@@ -4543,7 +4541,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>470</v>
       </c>
@@ -4566,7 +4564,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>471</v>
       </c>
@@ -4589,7 +4587,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>472</v>
       </c>
@@ -4612,7 +4610,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>473</v>
       </c>
@@ -4635,7 +4633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>474</v>
       </c>
@@ -4658,7 +4656,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>475</v>
       </c>
@@ -4681,7 +4679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>476</v>
       </c>
@@ -4704,7 +4702,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>477</v>
       </c>
@@ -4727,7 +4725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>495</v>
       </c>
@@ -4750,7 +4748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>507</v>
       </c>
@@ -4773,7 +4771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>510</v>
       </c>
@@ -4796,7 +4794,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>513</v>
       </c>
@@ -4819,7 +4817,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>516</v>
       </c>
@@ -4842,7 +4840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>519</v>
       </c>
@@ -4865,7 +4863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>522</v>
       </c>
@@ -4888,7 +4886,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>528</v>
       </c>
@@ -4911,7 +4909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>537</v>
       </c>
@@ -4934,7 +4932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>543</v>
       </c>
@@ -4957,7 +4955,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>549</v>
       </c>
@@ -4980,7 +4978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>552</v>
       </c>
@@ -5003,7 +5001,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>555</v>
       </c>
@@ -5026,7 +5024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>558</v>
       </c>
@@ -5049,7 +5047,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>561</v>
       </c>
@@ -5072,7 +5070,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>564</v>
       </c>
@@ -5095,7 +5093,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>567</v>
       </c>
@@ -5118,7 +5116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>570</v>
       </c>
@@ -5141,7 +5139,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>572</v>
       </c>
@@ -5164,7 +5162,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>573</v>
       </c>
@@ -5187,7 +5185,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>576</v>
       </c>
@@ -5210,7 +5208,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>579</v>
       </c>
@@ -5233,7 +5231,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>582</v>
       </c>
@@ -5256,7 +5254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>584</v>
       </c>
@@ -5279,7 +5277,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>585</v>
       </c>
@@ -5302,7 +5300,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>588</v>
       </c>
@@ -5313,19 +5311,19 @@
         <v>84</v>
       </c>
       <c r="D193" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F193" s="1">
+        <v>1</v>
+      </c>
+      <c r="G193" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E193" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F193" s="1">
-        <v>2</v>
-      </c>
-      <c r="G193" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>591</v>
       </c>
@@ -5345,10 +5343,10 @@
         <v>0</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>594</v>
       </c>
@@ -5359,19 +5357,19 @@
         <v>84</v>
       </c>
       <c r="D195" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F195" s="1">
+        <v>1</v>
+      </c>
+      <c r="G195" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E195" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F195" s="1">
-        <v>2</v>
-      </c>
-      <c r="G195" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>597</v>
       </c>
@@ -5391,10 +5389,10 @@
         <v>0</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>600</v>
       </c>
@@ -5405,19 +5403,19 @@
         <v>84</v>
       </c>
       <c r="D197" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F197" s="1">
+        <v>1</v>
+      </c>
+      <c r="G197" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E197" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F197" s="1">
-        <v>2</v>
-      </c>
-      <c r="G197" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>603</v>
       </c>
@@ -5437,10 +5435,10 @@
         <v>0</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>606</v>
       </c>
@@ -5463,7 +5461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>609</v>
       </c>
@@ -5486,7 +5484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>612</v>
       </c>
@@ -5494,22 +5492,22 @@
         <v>615</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D201" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F201" s="1">
+        <v>2</v>
+      </c>
+      <c r="G201" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E201" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F201" s="1">
-        <v>2</v>
-      </c>
-      <c r="G201" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>615</v>
       </c>
@@ -5517,7 +5515,7 @@
         <v>618</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D202" s="1">
         <v>5</v>
@@ -5529,10 +5527,10 @@
         <v>0</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>618</v>
       </c>
@@ -5540,22 +5538,22 @@
         <v>621</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D203" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F203" s="1">
+        <v>2</v>
+      </c>
+      <c r="G203" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E203" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F203" s="1">
-        <v>2</v>
-      </c>
-      <c r="G203" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>621</v>
       </c>
@@ -5563,7 +5561,7 @@
         <v>624</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D204" s="1">
         <v>5</v>
@@ -5575,10 +5573,10 @@
         <v>0</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>624</v>
       </c>
@@ -5586,22 +5584,22 @@
         <v>627</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D205" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F205" s="1">
+        <v>2</v>
+      </c>
+      <c r="G205" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E205" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F205" s="1">
-        <v>2</v>
-      </c>
-      <c r="G205" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>627</v>
       </c>
@@ -5609,7 +5607,7 @@
         <v>630</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D206" s="1">
         <v>5</v>
@@ -5621,10 +5619,10 @@
         <v>0</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>630</v>
       </c>
@@ -5632,7 +5630,7 @@
         <v>633</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D207" s="1">
         <v>5</v>
@@ -5647,7 +5645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>633</v>
       </c>
@@ -5655,22 +5653,22 @@
         <v>636</v>
       </c>
       <c r="C208" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D208" s="1">
+        <v>1</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F208" s="1">
+        <v>0</v>
+      </c>
+      <c r="G208" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D208" s="1">
-        <v>1</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F208" s="1">
-        <v>0</v>
-      </c>
-      <c r="G208" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>636</v>
       </c>
@@ -5678,7 +5676,7 @@
         <v>639</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D209" s="1">
         <v>5</v>
@@ -5693,7 +5691,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>639</v>
       </c>
@@ -5701,7 +5699,7 @@
         <v>642</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D210" s="1">
         <v>1</v>
@@ -5716,7 +5714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>642</v>
       </c>
@@ -5724,7 +5722,7 @@
         <v>645</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D211" s="1">
         <v>5</v>
@@ -5739,7 +5737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>645</v>
       </c>
@@ -5747,7 +5745,7 @@
         <v>648</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D212" s="1">
         <v>1</v>
@@ -5762,7 +5760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>648</v>
       </c>
@@ -5770,22 +5768,22 @@
         <v>651</v>
       </c>
       <c r="C213" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D213" s="1">
+        <v>1</v>
+      </c>
+      <c r="E213" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D213" s="1">
-        <v>1</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="F213" s="1">
         <v>0</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A214" s="5">
         <v>651</v>
       </c>
@@ -5793,22 +5791,22 @@
         <v>678</v>
       </c>
       <c r="C214" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D214" s="5">
+        <v>2</v>
+      </c>
+      <c r="E214" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F214" s="5">
+        <v>1</v>
+      </c>
+      <c r="G214" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D214" s="5">
-        <v>2</v>
-      </c>
-      <c r="E214" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F214" s="5">
-        <v>1</v>
-      </c>
-      <c r="G214" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="215" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>678</v>
       </c>
@@ -5831,7 +5829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>681</v>
       </c>
@@ -5854,7 +5852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>687</v>
       </c>
@@ -5877,7 +5875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>690</v>
       </c>
@@ -5900,7 +5898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>693</v>
       </c>
@@ -5923,7 +5921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>699</v>
       </c>
@@ -5946,7 +5944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>708</v>
       </c>
@@ -5969,7 +5967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>714</v>
       </c>
@@ -5992,7 +5990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>717</v>
       </c>
@@ -6015,7 +6013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>720</v>
       </c>
@@ -6038,7 +6036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>723</v>
       </c>
@@ -6061,7 +6059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>726</v>
       </c>
@@ -6084,7 +6082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>729</v>
       </c>
@@ -6107,7 +6105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>731</v>
       </c>
@@ -6130,7 +6128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>732</v>
       </c>
@@ -6153,7 +6151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>735</v>
       </c>
@@ -6176,7 +6174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>738</v>
       </c>
@@ -6199,7 +6197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>741</v>
       </c>
@@ -6222,7 +6220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>743</v>
       </c>
@@ -6245,7 +6243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>744</v>
       </c>
@@ -6268,7 +6266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>747</v>
       </c>
@@ -6291,7 +6289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>750</v>
       </c>
@@ -6314,7 +6312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>753</v>
       </c>
@@ -6337,7 +6335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>756</v>
       </c>
@@ -6360,7 +6358,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>759</v>
       </c>
@@ -6383,7 +6381,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>762</v>
       </c>
@@ -6406,7 +6404,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>771</v>
       </c>
@@ -6429,7 +6427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>777</v>
       </c>
@@ -6452,7 +6450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>780</v>
       </c>
@@ -6475,7 +6473,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>782</v>
       </c>
@@ -6498,7 +6496,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>783</v>
       </c>
@@ -6521,7 +6519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>788</v>
       </c>
@@ -6544,7 +6542,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>789</v>
       </c>
@@ -6567,7 +6565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>790</v>
       </c>
@@ -6590,7 +6588,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>791</v>
       </c>
@@ -6613,7 +6611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>792</v>
       </c>
@@ -6636,7 +6634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>810</v>
       </c>
@@ -6659,7 +6657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>816</v>
       </c>
@@ -6682,7 +6680,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>819</v>
       </c>
@@ -6705,7 +6703,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>821</v>
       </c>
@@ -6728,7 +6726,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>822</v>
       </c>
@@ -6751,7 +6749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>827</v>
       </c>
@@ -6774,7 +6772,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>828</v>
       </c>
@@ -6797,7 +6795,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>829</v>
       </c>
@@ -6820,7 +6818,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>830</v>
       </c>
@@ -6843,7 +6841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>831</v>
       </c>
@@ -6866,7 +6864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>834</v>
       </c>
@@ -6889,7 +6887,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>837</v>
       </c>
@@ -6912,7 +6910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>840</v>
       </c>
@@ -6935,7 +6933,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>843</v>
       </c>
@@ -6958,7 +6956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>844</v>
       </c>
@@ -6981,7 +6979,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>845</v>
       </c>
@@ -7004,7 +7002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>846</v>
       </c>
@@ -7027,7 +7025,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>847</v>
       </c>
@@ -7050,7 +7048,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>848</v>
       </c>
@@ -7073,7 +7071,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>849</v>
       </c>
@@ -7096,7 +7094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>850</v>
       </c>
@@ -7119,7 +7117,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>851</v>
       </c>
@@ -7142,7 +7140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>852</v>
       </c>
@@ -7165,7 +7163,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>853</v>
       </c>
@@ -7188,7 +7186,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>854</v>
       </c>
@@ -7211,7 +7209,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>855</v>
       </c>
@@ -7234,7 +7232,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>856</v>
       </c>
@@ -7257,7 +7255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>857</v>
       </c>
@@ -7280,7 +7278,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>858</v>
       </c>
@@ -7303,7 +7301,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>859</v>
       </c>
@@ -7326,7 +7324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>860</v>
       </c>
@@ -7349,7 +7347,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>861</v>
       </c>
@@ -7372,7 +7370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>862</v>
       </c>
@@ -7395,7 +7393,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>863</v>
       </c>
@@ -7418,7 +7416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>864</v>
       </c>
@@ -7441,7 +7439,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>867</v>
       </c>
@@ -7464,7 +7462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>885</v>
       </c>
@@ -7487,7 +7485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>900</v>
       </c>
@@ -7510,7 +7508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>903</v>
       </c>
@@ -7533,7 +7531,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>906</v>
       </c>
@@ -7556,7 +7554,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>909</v>
       </c>
@@ -7579,7 +7577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>912</v>
       </c>
@@ -7602,7 +7600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>915</v>
       </c>
@@ -7610,7 +7608,7 @@
         <v>921</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D293" s="1">
         <v>1</v>
@@ -7625,7 +7623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>921</v>
       </c>
@@ -7633,7 +7631,7 @@
         <v>930</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D294" s="1">
         <v>2</v>
@@ -7648,7 +7646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>930</v>
       </c>
@@ -7656,7 +7654,7 @@
         <v>936</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>3</v>
@@ -7671,7 +7669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>936</v>
       </c>
@@ -7679,22 +7677,22 @@
         <v>939</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D296" s="1">
         <v>5</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F296" s="1">
         <v>2</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>939</v>
       </c>
@@ -7702,22 +7700,22 @@
         <v>942</v>
       </c>
       <c r="C297" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D297" s="1">
+        <v>1</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F297" s="1">
+        <v>1</v>
+      </c>
+      <c r="G297" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D297" s="1">
-        <v>1</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F297" s="1">
-        <v>1</v>
-      </c>
-      <c r="G297" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>942</v>
       </c>
@@ -7725,7 +7723,7 @@
         <v>945</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D298" s="1">
         <v>7</v>
@@ -7737,10 +7735,10 @@
         <v>1</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>945</v>
       </c>
@@ -7748,22 +7746,22 @@
         <v>948</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D299" s="1">
         <v>1</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F299" s="1">
         <v>1</v>
       </c>
       <c r="G299" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>948</v>
       </c>
@@ -7771,22 +7769,22 @@
         <v>951</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F300" s="1">
         <v>1</v>
       </c>
       <c r="G300" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>951</v>
       </c>
@@ -7794,22 +7792,22 @@
         <v>954</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D301" s="1">
         <v>2</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F301" s="1">
         <v>1</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>954</v>
       </c>
@@ -7817,7 +7815,7 @@
         <v>960</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D302" s="2" t="s">
         <v>3</v>
@@ -7832,7 +7830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>960</v>
       </c>
@@ -7840,22 +7838,22 @@
         <v>965</v>
       </c>
       <c r="C303" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D303" s="1">
+        <v>1</v>
+      </c>
+      <c r="E303" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D303" s="1">
-        <v>1</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F303" s="1">
         <v>2</v>
       </c>
       <c r="G303" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>965</v>
       </c>
@@ -7863,7 +7861,7 @@
         <v>966</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D304" s="1">
         <v>5</v>
@@ -7878,7 +7876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>966</v>
       </c>
@@ -7886,7 +7884,7 @@
         <v>972</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D305" s="1">
         <v>1</v>
@@ -7901,7 +7899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>972</v>
       </c>
@@ -7909,7 +7907,7 @@
         <v>981</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D306" s="1">
         <v>2</v>
@@ -7924,7 +7922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>981</v>
       </c>
@@ -7932,7 +7930,7 @@
         <v>987</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D307" s="2" t="s">
         <v>3</v>
@@ -7947,7 +7945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>987</v>
       </c>
@@ -7955,22 +7953,22 @@
         <v>989</v>
       </c>
       <c r="C308" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D308" s="1">
+        <v>1</v>
+      </c>
+      <c r="E308" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D308" s="1">
-        <v>1</v>
-      </c>
-      <c r="E308" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F308" s="1">
         <v>2</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>989</v>
       </c>
@@ -7978,10 +7976,10 @@
         <v>990</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E309" s="1" t="s">
         <v>4</v>
@@ -7990,10 +7988,10 @@
         <v>1</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>990</v>
       </c>
@@ -8001,22 +7999,22 @@
         <v>992</v>
       </c>
       <c r="C310" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D310" s="1">
+        <v>1</v>
+      </c>
+      <c r="E310" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D310" s="1">
-        <v>1</v>
-      </c>
-      <c r="E310" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F310" s="1">
         <v>2</v>
       </c>
       <c r="G310" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>992</v>
       </c>
@@ -8024,10 +8022,10 @@
         <v>993</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E311" s="1" t="s">
         <v>4</v>
@@ -8036,10 +8034,10 @@
         <v>1</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>993</v>
       </c>
@@ -8047,22 +8045,22 @@
         <v>996</v>
       </c>
       <c r="C312" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D312" s="1">
+        <v>1</v>
+      </c>
+      <c r="E312" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D312" s="1">
-        <v>1</v>
-      </c>
-      <c r="E312" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F312" s="1">
         <v>2</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>996</v>
       </c>
@@ -8070,7 +8068,7 @@
         <v>999</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D313" s="1">
         <v>5</v>
@@ -8085,7 +8083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>999</v>
       </c>
@@ -8093,7 +8091,7 @@
         <v>1002</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D314" s="1">
         <v>1</v>
@@ -8108,7 +8106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>1002</v>
       </c>
@@ -8116,7 +8114,7 @@
         <v>1005</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D315" s="1">
         <v>5</v>
@@ -8131,7 +8129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>1005</v>
       </c>
@@ -8139,7 +8137,7 @@
         <v>1008</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D316" s="1">
         <v>1</v>
@@ -8154,7 +8152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>1008</v>
       </c>
@@ -8162,7 +8160,7 @@
         <v>1011</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D317" s="1">
         <v>5</v>
@@ -8177,7 +8175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>1011</v>
       </c>
@@ -8185,7 +8183,7 @@
         <v>1019</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D318" s="1">
         <v>1</v>
@@ -8200,7 +8198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>1019</v>
       </c>
@@ -8208,7 +8206,7 @@
         <v>1020</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D319" s="1">
         <v>5</v>
@@ -8223,7 +8221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>1020</v>
       </c>
@@ -8231,7 +8229,7 @@
         <v>1023</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D320" s="1">
         <v>1</v>

</xml_diff>